<commit_message>
saving pregnant women into mongo db
</commit_message>
<xml_diff>
--- a/backend/xlsForms/household_visit.xlsx
+++ b/backend/xlsForms/household_visit.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="650">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -430,9 +430,6 @@
   </si>
   <si>
     <t xml:space="preserve">When was your last menstrual period?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${visit_objective}!=’followup’</t>
   </si>
   <si>
     <t xml:space="preserve">select_multiple danger_signs</t>
@@ -715,32 +712,7 @@
     <t xml:space="preserve">Rule out Neonatal/ children danger sign</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">delivery_outcome</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}!=’dead’</t>
-    </r>
+    <t xml:space="preserve">${delivery_outcome}!=’dead’</t>
   </si>
   <si>
     <t xml:space="preserve">baby_back_post_clin</t>
@@ -848,23 +820,7 @@
     <t xml:space="preserve">note_add_all_children</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Add all children age</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> and other details</t>
-    </r>
+    <t xml:space="preserve">Add all children age and other details</t>
   </si>
   <si>
     <t xml:space="preserve">rp_children_under_5</t>
@@ -2027,7 +1983,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0_);\(#,##0\)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -2061,11 +2017,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2117,7 +2068,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2142,15 +2093,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2173,8 +2120,8 @@
   </sheetPr>
   <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A104" activeCellId="0" sqref="104:104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E65" activeCellId="0" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2964,7 +2911,7 @@
       <c r="B59" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="J59" s="6" t="s">
+      <c r="J59" s="1" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3020,6 +2967,9 @@
       <c r="C63" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="E63" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G63" s="1" t="s">
         <v>130</v>
       </c>
@@ -3034,6 +2984,9 @@
       <c r="C64" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="E64" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G64" s="1" t="s">
         <v>130</v>
       </c>
@@ -3049,29 +3002,29 @@
         <v>135</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>24</v>
@@ -3082,13 +3035,13 @@
         <v>61</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,10 +3049,10 @@
         <v>122</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3107,10 +3060,10 @@
         <v>133</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3118,10 +3071,10 @@
         <v>133</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3129,10 +3082,10 @@
         <v>133</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3140,10 +3093,10 @@
         <v>133</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3156,24 +3109,24 @@
         <v>122</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="G75" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,24 +3134,24 @@
         <v>37</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="G77" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>24</v>
@@ -3206,30 +3159,30 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>24</v>
@@ -3237,19 +3190,19 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3257,10 +3210,10 @@
         <v>61</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>64</v>
@@ -3271,10 +3224,10 @@
         <v>122</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3282,10 +3235,10 @@
         <v>122</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3293,10 +3246,10 @@
         <v>122</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3306,13 +3259,13 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>24</v>
@@ -3323,13 +3276,13 @@
         <v>37</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="G88" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3339,7 +3292,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3347,10 +3300,10 @@
         <v>116</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J91" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="J91" s="6" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3358,13 +3311,13 @@
         <v>61</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="G92" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,10 +3325,10 @@
         <v>122</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3383,21 +3336,21 @@
         <v>133</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>24</v>
@@ -3405,13 +3358,13 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>24</v>
@@ -3422,13 +3375,13 @@
         <v>37</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="G97" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3436,13 +3389,13 @@
         <v>37</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="G98" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3450,24 +3403,24 @@
         <v>133</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="G99" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3475,13 +3428,13 @@
         <v>122</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="G101" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3489,21 +3442,21 @@
         <v>116</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J102" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="J102" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>24</v>
@@ -3511,49 +3464,49 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="J105" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="J105" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>24</v>
@@ -3561,33 +3514,33 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="G109" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3595,13 +3548,13 @@
         <v>37</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="G110" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3609,24 +3562,24 @@
         <v>122</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="G111" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3634,24 +3587,24 @@
         <v>37</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="G113" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3659,10 +3612,10 @@
         <v>122</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3670,10 +3623,10 @@
         <v>122</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3683,7 +3636,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3691,13 +3644,13 @@
         <v>61</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="G119" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3705,21 +3658,21 @@
         <v>122</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>24</v>
@@ -3730,10 +3683,10 @@
         <v>122</v>
       </c>
       <c r="B122" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3741,10 +3694,10 @@
         <v>116</v>
       </c>
       <c r="B123" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J123" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="J123" s="1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3752,21 +3705,21 @@
         <v>55</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="C125" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3774,24 +3727,24 @@
         <v>133</v>
       </c>
       <c r="B126" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="G126" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B127" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>24</v>
@@ -3799,16 +3752,16 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="C128" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="G128" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3816,18 +3769,18 @@
         <v>122</v>
       </c>
       <c r="B129" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="G129" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3840,10 +3793,10 @@
         <v>61</v>
       </c>
       <c r="B132" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3851,21 +3804,21 @@
         <v>122</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B134" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3873,13 +3826,13 @@
         <v>55</v>
       </c>
       <c r="B135" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="G135" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3887,10 +3840,10 @@
         <v>116</v>
       </c>
       <c r="B136" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="J136" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="J136" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3898,21 +3851,21 @@
         <v>55</v>
       </c>
       <c r="B137" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="C138" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3920,29 +3873,29 @@
         <v>37</v>
       </c>
       <c r="B139" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C139" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="G139" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>24</v>
@@ -3950,13 +3903,13 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="C142" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>308</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>24</v>
@@ -3967,24 +3920,24 @@
         <v>37</v>
       </c>
       <c r="B143" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C143" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="G143" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="C144" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3992,13 +3945,13 @@
         <v>37</v>
       </c>
       <c r="B145" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C145" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="G145" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4008,13 +3961,13 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="C147" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>24</v>
@@ -4038,8 +3991,8 @@
   </sheetPr>
   <dimension ref="A1:D216"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="1" sqref="104:104 A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A194" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D216" activeCellId="0" sqref="D216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4052,7 +4005,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4061,7 +4014,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4069,10 +4022,10 @@
         <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4080,10 +4033,10 @@
         <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4091,18 +4044,18 @@
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>330</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>66</v>
@@ -4110,10 +4063,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>68</v>
@@ -4124,10 +4077,10 @@
         <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4135,10 +4088,10 @@
         <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>334</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4146,10 +4099,10 @@
         <v>59</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4157,2434 +4110,2434 @@
         <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>373</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>399</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B46" s="7" t="n">
+        <v>199</v>
+      </c>
+      <c r="B46" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B47" s="7" t="n">
+        <v>199</v>
+      </c>
+      <c r="B47" s="6" t="n">
         <v>2</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B48" s="7" t="n">
+        <v>199</v>
+      </c>
+      <c r="B48" s="6" t="n">
         <v>3</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>441</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>447</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>451</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>472</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>477</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>490</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>502</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>504</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>506</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>514</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>516</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>525</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>532</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>538</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B122" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B123" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>544</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B125" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B126" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>548</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B127" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>551</v>
-      </c>
       <c r="C128" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B144" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>567</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>578</v>
-      </c>
       <c r="C153" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B189" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C189" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="C189" s="1" t="s">
-        <v>615</v>
-      </c>
       <c r="D189" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B204" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="C204" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="C204" s="1" t="s">
-        <v>631</v>
-      </c>
       <c r="D204" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B205" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="C205" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="C205" s="1" t="s">
-        <v>633</v>
-      </c>
       <c r="D205" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B210" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="B210" s="1" t="s">
-        <v>639</v>
-      </c>
       <c r="C210" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6592,27 +6545,27 @@
         <v>34</v>
       </c>
       <c r="B215" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C215" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="C215" s="1" t="s">
-        <v>645</v>
-      </c>
       <c r="D215" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B216" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C216" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="C216" s="1" t="s">
-        <v>645</v>
-      </c>
       <c r="D216" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -6634,7 +6587,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="1" sqref="104:104 I30"/>
+      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6644,19 +6597,19 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>647</v>
       </c>
-      <c r="B1" s="8" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>649</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>